<commit_message>
Martin & Daniel nicknams & task.
</commit_message>
<xml_diff>
--- a/MaintainProjectTasks.xlsx
+++ b/MaintainProjectTasks.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="37">
   <si>
     <t xml:space="preserve">Task</t>
   </si>
@@ -145,6 +145,12 @@
   </si>
   <si>
     <t xml:space="preserve">Add seed numbers to brackets. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Villanova bug</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Martin&amp;Daniel</t>
   </si>
   <si>
     <t xml:space="preserve">Add minimum password length. </t>
@@ -262,19 +268,16 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="128"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="128"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="128"/>
     </font>
     <font>
       <b val="true"/>
@@ -367,7 +370,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="7" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="9" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -571,15 +574,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="65.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="65.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="29.71"/>
@@ -650,6 +653,17 @@
       </c>
       <c r="B8" s="0" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -699,7 +713,7 @@
     </row>
     <row r="2" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>5</v>
@@ -707,7 +721,7 @@
     </row>
     <row r="3" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>5</v>
@@ -715,7 +729,7 @@
     </row>
     <row r="4" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>5</v>
@@ -723,7 +737,7 @@
     </row>
     <row r="5" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>5</v>
@@ -731,7 +745,7 @@
     </row>
     <row r="6" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>5</v>
@@ -742,7 +756,7 @@
     </row>
     <row r="8" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>9</v>
@@ -753,7 +767,7 @@
     </row>
     <row r="10" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>14</v>
@@ -761,7 +775,7 @@
     </row>
     <row r="11" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>14</v>
@@ -769,7 +783,7 @@
     </row>
     <row r="12" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>14</v>
@@ -777,7 +791,7 @@
     </row>
     <row r="13" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B13" s="0" t="s">
         <v>14</v>
@@ -785,7 +799,7 @@
     </row>
     <row r="14" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B14" s="0" t="s">
         <v>14</v>
@@ -793,7 +807,7 @@
     </row>
     <row r="15" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B15" s="0" t="s">
         <v>14</v>
@@ -801,7 +815,7 @@
     </row>
     <row r="16" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B16" s="0" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
Fixed the excel document again
</commit_message>
<xml_diff>
--- a/MaintainProjectTasks.xlsx
+++ b/MaintainProjectTasks.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Bug Fixes" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="38">
   <si>
     <t xml:space="preserve">Task</t>
   </si>
@@ -64,6 +64,9 @@
     <t xml:space="preserve">Trouble finalizing. Is it related to Villanova? </t>
   </si>
   <si>
+    <t xml:space="preserve">Martin&amp;Daniel</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="7"/>
@@ -151,12 +154,6 @@
   </si>
   <si>
     <t xml:space="preserve">Add seed numbers to brackets. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Villanova</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Martin&amp;Daniel</t>
   </si>
   <si>
     <t xml:space="preserve">Add minimum password length. </t>
@@ -376,7 +373,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="9" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="12" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -462,15 +459,15 @@
   </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="30.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.67"/>
   </cols>
@@ -497,17 +494,20 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="19.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="C3" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="59.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>5</v>
@@ -518,34 +518,34 @@
     </row>
     <row r="6" customFormat="false" ht="19.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="19.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="0" t="s">
         <v>10</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="19.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="19.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="11.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -553,10 +553,10 @@
     </row>
     <row r="11" customFormat="false" ht="19.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -577,14 +577,14 @@
   </sheetPr>
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="65.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="29.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.67"/>
@@ -606,7 +606,7 @@
     </row>
     <row r="2" customFormat="false" ht="19.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>5</v>
@@ -617,38 +617,38 @@
     </row>
     <row r="4" customFormat="false" ht="19.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="19.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="19.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -656,23 +656,14 @@
     </row>
     <row r="8" customFormat="false" ht="19.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>25</v>
-      </c>
-    </row>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -720,7 +711,7 @@
     </row>
     <row r="2" customFormat="false" ht="19.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>5</v>
@@ -728,7 +719,7 @@
     </row>
     <row r="3" customFormat="false" ht="19.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>5</v>
@@ -736,7 +727,7 @@
     </row>
     <row r="4" customFormat="false" ht="19.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>5</v>
@@ -744,7 +735,7 @@
     </row>
     <row r="5" customFormat="false" ht="19.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>5</v>
@@ -752,7 +743,7 @@
     </row>
     <row r="6" customFormat="false" ht="39.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>5</v>
@@ -763,10 +754,10 @@
     </row>
     <row r="8" customFormat="false" ht="19.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -774,58 +765,58 @@
     </row>
     <row r="10" customFormat="false" ht="19.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="19.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="19.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="19.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="39.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="19.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added my nickname and bug choice
</commit_message>
<xml_diff>
--- a/MaintainProjectTasks.xlsx
+++ b/MaintainProjectTasks.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17127"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Harold\Cs225\maintainasgn\CS225-March-Madness\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\niuti\Desktop\MassBay\CS225\MarchMadness\CS225-March-Madness\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FAA5C6F-2EA2-4A8B-B8D8-D1161002798A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bug Fixes" sheetId="1" r:id="rId1"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="41">
   <si>
     <t>Task</t>
   </si>
@@ -258,11 +259,18 @@
   <si>
     <t>Nikolas</t>
   </si>
+  <si>
+    <t>Ana Gorohovschi</t>
+  </si>
+  <si>
+    <t>MarchMadnessGUI.java
+SerializeTest.java</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -302,7 +310,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -310,11 +318,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -333,6 +356,20 @@
       <alignment horizontal="left" vertical="center" indent="12"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -714,11 +751,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -731,100 +768,125 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="42" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="11" t="s">
         <v>5</v>
       </c>
+      <c r="C2" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="3" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="11" t="s">
         <v>7</v>
       </c>
+      <c r="D3" s="11"/>
     </row>
     <row r="4" spans="1:4" ht="63" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="11" t="s">
         <v>5</v>
       </c>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
     </row>
     <row r="5" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
+      <c r="A5" s="10"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
     </row>
     <row r="6" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="11" t="s">
         <v>10</v>
       </c>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
     </row>
     <row r="7" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="11" t="s">
         <v>10</v>
       </c>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
     </row>
     <row r="8" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="11" t="s">
         <v>10</v>
       </c>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
     </row>
     <row r="9" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="11" t="s">
         <v>10</v>
       </c>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
     </row>
     <row r="10" spans="1:4" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
+      <c r="A10" s="10"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
     </row>
     <row r="11" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="11" t="s">
         <v>15</v>
       </c>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -919,10 +981,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added peter's file info
</commit_message>
<xml_diff>
--- a/MaintainProjectTasks.xlsx
+++ b/MaintainProjectTasks.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thien\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pbels\CS225-March-Madness\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CB50A81-D611-4526-B16C-3D5F144C98D7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bug Fixes" sheetId="1" r:id="rId1"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="45">
   <si>
     <t>Task</t>
   </si>
@@ -271,11 +272,17 @@
   <si>
     <t>Thien</t>
   </si>
+  <si>
+    <t>Peter</t>
+  </si>
+  <si>
+    <t>MarchMadnessGUI, Bracket</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -756,7 +763,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -891,11 +898,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -928,6 +935,12 @@
       <c r="B2" t="s">
         <v>5</v>
       </c>
+      <c r="C2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="3" spans="1:4" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
@@ -992,7 +1005,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">

</xml_diff>

<commit_message>
Changed C task to TournamentInfo
</commit_message>
<xml_diff>
--- a/MaintainProjectTasks.xlsx
+++ b/MaintainProjectTasks.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\j_mitchell22\CS225-March-Madness\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmitc\CS225-March-Madness\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Bug Fixes" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="62">
   <si>
     <t>Task</t>
   </si>
@@ -65,10 +65,20 @@
     <t>A</t>
   </si>
   <si>
+    <t>Ana Gorohovschi</t>
+  </si>
+  <si>
+    <t>MarchMadnessGUI.java
+SerializeTest.java</t>
+  </si>
+  <si>
     <t xml:space="preserve">Trouble finalizing. Is it related to Villanova? </t>
   </si>
   <si>
-    <t>Martin&amp;Daniel</t>
+    <t>Martin&amp;Daniel&amp;Christian</t>
+  </si>
+  <si>
+    <t>resetSubtree() in Bracket.java</t>
   </si>
   <si>
     <r>
@@ -93,6 +103,12 @@
     </r>
   </si>
   <si>
+    <t>Mike S.</t>
+  </si>
+  <si>
+    <t>BracketPane.java</t>
+  </si>
+  <si>
     <t xml:space="preserve">Error when finalizing “null.ser(access denied)”. </t>
   </si>
   <si>
@@ -121,12 +137,30 @@
     </r>
   </si>
   <si>
+    <t>Benjamin &amp; Ana</t>
+  </si>
+  <si>
+    <t>Bracket.java</t>
+  </si>
+  <si>
     <t>Once the simulation has been completed, user can’t log out?</t>
   </si>
   <si>
+    <t>Vrej</t>
+  </si>
+  <si>
+    <t>MarchMadnessGUI.java</t>
+  </si>
+  <si>
     <t xml:space="preserve">The user can change a finalize bracket (user can cheat!). </t>
   </si>
   <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Note: Bug not replicable</t>
+  </si>
+  <si>
     <t xml:space="preserve">The system allows the user to create unlimited users. </t>
   </si>
   <si>
@@ -136,6 +170,12 @@
     <t xml:space="preserve">Add password encryption. </t>
   </si>
   <si>
+    <t>Peter</t>
+  </si>
+  <si>
+    <t>MarchMadnessGUI, Bracket</t>
+  </si>
+  <si>
     <t>Remove user accounts.</t>
   </si>
   <si>
@@ -157,10 +197,16 @@
     <t>Resize the full bracket without side scrolling.</t>
   </si>
   <si>
+    <t>Thien</t>
+  </si>
+  <si>
     <t xml:space="preserve">Add seed numbers to brackets. </t>
   </si>
   <si>
     <t xml:space="preserve">Add minimum password length. </t>
+  </si>
+  <si>
+    <t>Nikolas</t>
   </si>
   <si>
     <r>
@@ -210,13 +256,31 @@
     </r>
   </si>
   <si>
+    <t>Ben</t>
+  </si>
+  <si>
+    <t>Uml</t>
+  </si>
+  <si>
     <t>Implement the simple tutorial. This can be helpful for checking the teams states</t>
   </si>
   <si>
+    <t>Devin/Paul</t>
+  </si>
+  <si>
     <t xml:space="preserve">Add a warning confirmation dialog when the user is about to finalize.  </t>
   </si>
   <si>
+    <t>Gennadiy</t>
+  </si>
+  <si>
+    <t>MarchmadnessGUI</t>
+  </si>
+  <si>
     <t>Resize (Northern Kentucky, South Dakota State)</t>
+  </si>
+  <si>
+    <t>initialmatches.txt, teaminfo.txt</t>
   </si>
   <si>
     <r>
@@ -244,9 +308,15 @@
     <t>Change orientation of choose division buttons.</t>
   </si>
   <si>
+    <t xml:space="preserve">Bracketpane  </t>
+  </si>
+  <si>
     <t>Final two teams should be on top of the platform.</t>
   </si>
   <si>
+    <t>BracketPane</t>
+  </si>
+  <si>
     <t>Place buttons in one area (drop dpwn menu for the users instead of button)</t>
   </si>
   <si>
@@ -256,33 +326,14 @@
     <t xml:space="preserve">“user winning teams” selection for the simulation board </t>
   </si>
   <si>
-    <t>Nikolas</t>
-  </si>
-  <si>
-    <t>Ana Gorohovschi</t>
-  </si>
-  <si>
-    <t>MarchMadnessGUI.java
-SerializeTest.java</t>
-  </si>
-  <si>
-    <t>Devin/Paul</t>
-  </si>
-  <si>
-    <t>Thien</t>
-  </si>
-  <si>
-    <t>Peter</t>
-  </si>
-  <si>
-    <t>MarchMadnessGUI, Bracket</t>
+    <t>TournamentInfo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -312,6 +363,13 @@
       <family val="4"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -331,16 +389,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -348,39 +406,40 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="12"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="15"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -483,7 +542,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -495,7 +554,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -763,136 +822,158 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="87" style="1" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="22.85546875" customWidth="1"/>
-    <col min="4" max="4" width="30.140625" customWidth="1"/>
-    <col min="5" max="1025" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="22.88671875" customWidth="1"/>
+    <col min="4" max="4" width="30.109375" customWidth="1"/>
+    <col min="5" max="5" width="26.5546875" customWidth="1"/>
+    <col min="6" max="1025" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:5" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="42" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+    <row r="2" spans="1:5" ht="39.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
+      <c r="C2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="D2" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="19.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="11"/>
-    </row>
-    <row r="4" spans="1:4" ht="63" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="11" t="s">
+      <c r="C3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="59.4" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-    </row>
-    <row r="5" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-    </row>
-    <row r="6" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-    </row>
-    <row r="7" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-    </row>
-    <row r="8" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
+      <c r="C4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-    </row>
-    <row r="9" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
+      <c r="D4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-    </row>
-    <row r="10" spans="1:4" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="10"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-    </row>
-    <row r="11" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
+    </row>
+    <row r="5" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="5"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+    </row>
+    <row r="6" spans="1:5" ht="19.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B6" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+    </row>
+    <row r="7" spans="1:5" ht="19.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="19.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="19.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="5"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+    </row>
+    <row r="11" spans="1:5" ht="19.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
@@ -901,106 +982,106 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="65.7109375" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" customWidth="1"/>
-    <col min="4" max="4" width="29.7109375" customWidth="1"/>
-    <col min="5" max="1025" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="65.6640625" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" customWidth="1"/>
+    <col min="3" max="3" width="13.109375" customWidth="1"/>
+    <col min="4" max="4" width="29.6640625" customWidth="1"/>
+    <col min="5" max="1025" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:4" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>16</v>
+    <row r="2" spans="1:4" ht="19.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
+        <v>27</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="D2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
-    </row>
-    <row r="4" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>17</v>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="10"/>
+    </row>
+    <row r="4" spans="1:4" ht="19.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="10" t="s">
+        <v>30</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>20</v>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="19.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>23</v>
+        <v>34</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="19.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="10" t="s">
+        <v>36</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>42</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
-    </row>
-    <row r="8" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>24</v>
+        <v>37</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="10"/>
+    </row>
+    <row r="8" spans="1:4" ht="19.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="10" t="s">
+        <v>38</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="D8" t="s">
-        <v>19</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1011,155 +1092,186 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="89.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125"/>
-    <col min="3" max="3" width="15.5703125" customWidth="1"/>
-    <col min="4" max="4" width="46.28515625" customWidth="1"/>
-    <col min="5" max="1025" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="89.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.44140625"/>
+    <col min="3" max="3" width="15.5546875" customWidth="1"/>
+    <col min="4" max="4" width="46.33203125" customWidth="1"/>
+    <col min="5" max="1025" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:5" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>25</v>
+    <row r="2" spans="1:5" ht="19.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="12" t="s">
+        <v>39</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>26</v>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="19.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="13" t="s">
+        <v>41</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>27</v>
+    <row r="4" spans="1:5" ht="19.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="12" t="s">
+        <v>42</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>28</v>
+    <row r="5" spans="1:5" ht="19.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="13" t="s">
+        <v>43</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="42" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>29</v>
+      <c r="C5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="39.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="12" t="s">
+        <v>46</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-    </row>
-    <row r="8" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="13"/>
+    </row>
+    <row r="8" spans="1:5" ht="19.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="12" t="s">
+        <v>48</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-    </row>
-    <row r="10" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>31</v>
+        <v>15</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E8" s="14"/>
+    </row>
+    <row r="9" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="13"/>
+    </row>
+    <row r="10" spans="1:5" ht="19.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="12" t="s">
+        <v>51</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>32</v>
+        <v>26</v>
+      </c>
+      <c r="C10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="19.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="13" t="s">
+        <v>53</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>33</v>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="19.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="12" t="s">
+        <v>54</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>34</v>
+        <v>26</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="19.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="12" t="s">
+        <v>56</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="42" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
-        <v>35</v>
+        <v>26</v>
+      </c>
+      <c r="C13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="39.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="12" t="s">
+        <v>58</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>36</v>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="19.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="12" t="s">
+        <v>59</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
-        <v>37</v>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="12" t="s">
+        <v>60</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>